<commit_message>
Ver 2.0 of board.
Also major advances in code.
</commit_message>
<xml_diff>
--- a/main_board/bom/lcsc/main_board_lcsc.xlsx
+++ b/main_board/bom/lcsc/main_board_lcsc.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shann\Dropbox\moog\bonkulator\main_board\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shann\Dropbox\moog\bonkulator\main_board\bom\lcsc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{3D18E9E4-4A02-4B7E-A1CE-AE0AFDEA24EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{BAEFF211-87F7-4290-A82F-EEA204AAF6F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="105">
   <si>
     <t>Reference</t>
   </si>
@@ -43,12 +43,21 @@
     <t>100uF</t>
   </si>
   <si>
+    <t>Capacitor_SMD:CP_Elec_6.3x5.4_Nichicon</t>
+  </si>
+  <si>
+    <t>C2887276</t>
+  </si>
+  <si>
     <t xml:space="preserve">C11 C12 C13 C26 </t>
   </si>
   <si>
     <t>10nF</t>
   </si>
   <si>
+    <t>Capacitor_SMD:C_0805_2012Metric_Pad1.18x1.45mm_HandSolder</t>
+  </si>
+  <si>
     <t>C83170</t>
   </si>
   <si>
@@ -58,16 +67,19 @@
     <t>2.2uF</t>
   </si>
   <si>
+    <t>Capacitor_Tantalum_SMD:CP_EIA-2012-15_AVX-P</t>
+  </si>
+  <si>
     <t>C273666</t>
   </si>
   <si>
-    <t xml:space="preserve">C3 C4 C5 C6 C8 C9 C10 C15 C16 C17 C18 C19 C20 C21 C22 C23 C24 C25 C27 C28 C29 C30 C31 C32 C33 </t>
+    <t xml:space="preserve">C3 C4 C5 C6 C8 C9 C10 C15 C16 C17 C18 C19 C20 C21 C22 C23 C24 C25 C27 C28 C29 C30 C32 C33 C34 C35 C36 C37 C38 C39 C40 C41 C42 </t>
   </si>
   <si>
     <t>100nF</t>
   </si>
   <si>
-    <t>C2909631</t>
+    <t>C49678</t>
   </si>
   <si>
     <t xml:space="preserve">C7 </t>
@@ -85,6 +97,9 @@
     <t>BAT46</t>
   </si>
   <si>
+    <t>Diode_SMD:D_0805_2012Metric_Pad1.15x1.40mm_HandSolder</t>
+  </si>
+  <si>
     <t>C123899</t>
   </si>
   <si>
@@ -94,12 +109,39 @@
     <t>Conn_01x15_Female</t>
   </si>
   <si>
-    <t xml:space="preserve">R1 R2 R3 R4 R32 R37 </t>
+    <t>sputterizer:ArduinoConnector</t>
+  </si>
+  <si>
+    <t>C124408</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J6 </t>
+  </si>
+  <si>
+    <t>EU Power</t>
+  </si>
+  <si>
+    <t>Connector_PinHeader_2.54mm:PinHeader_2x05_P2.54mm_Vertical</t>
+  </si>
+  <si>
+    <t>C115170</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J7 </t>
+  </si>
+  <si>
+    <t>Expansion Header</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R1 R2 R3 R4 R32 R37 R56 R57 R58 R59 R60 R61 R66 R67 R68 R81 R82 R83 R84 R93 R94 R95 R96 R109 R110 R111 R112 R121 R122 R123 R124 R125 R126 R127 R128 </t>
   </si>
   <si>
     <t>10K</t>
   </si>
   <si>
+    <t>Resistor_SMD:R_0805_2012Metric_Pad1.20x1.40mm_HandSolder</t>
+  </si>
+  <si>
     <t>C138260</t>
   </si>
   <si>
@@ -133,10 +175,13 @@
     <t xml:space="preserve">R24 R25 R26 R27 R28 R33 R52 R53 R54 R55 </t>
   </si>
   <si>
-    <t>C2681637</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R5 R6 R7 R8 R38 R39 </t>
+    <t>332K .1%</t>
+  </si>
+  <si>
+    <t>C228750</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R5 R6 R7 R8 R38 R39 R89 R90 R91 R92 R117 R118 R119 R120 </t>
   </si>
   <si>
     <t>1K</t>
@@ -145,6 +190,60 @@
     <t>C100047</t>
   </si>
   <si>
+    <t xml:space="preserve">R62 R63 </t>
+  </si>
+  <si>
+    <t>1M</t>
+  </si>
+  <si>
+    <t>C229154</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R64 R65 </t>
+  </si>
+  <si>
+    <t>100K</t>
+  </si>
+  <si>
+    <t>C100049</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R69 R70 R71 R72 R97 R98 R99 R100 </t>
+  </si>
+  <si>
+    <t>1.00M</t>
+  </si>
+  <si>
+    <t>C107700</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R73 R74 R75 R76 R101 R102 R103 R104 </t>
+  </si>
+  <si>
+    <t>750K</t>
+  </si>
+  <si>
+    <t>C137408</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R77 R78 R79 R80 R105 R106 R107 R108 </t>
+  </si>
+  <si>
+    <t>3.32M</t>
+  </si>
+  <si>
+    <t>C422748</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R85 R86 R87 R88 R113 R114 R115 R116 </t>
+  </si>
+  <si>
+    <t>2.2K</t>
+  </si>
+  <si>
+    <t>C26017</t>
+  </si>
+  <si>
     <t xml:space="preserve">R9 </t>
   </si>
   <si>
@@ -154,12 +253,15 @@
     <t>C473320</t>
   </si>
   <si>
-    <t xml:space="preserve">U1 U2 U5 U8 U9 U10 U12 </t>
+    <t xml:space="preserve">U1 U2 U4 U5 U8 U9 U10 U12 U14 U17 U18 </t>
   </si>
   <si>
     <t>TLV2172IDR</t>
   </si>
   <si>
+    <t>Package_SO:SOIC-8-1EP_3.9x4.9mm_P1.27mm_EP2.29x3mm</t>
+  </si>
+  <si>
     <t>C129149</t>
   </si>
   <si>
@@ -169,13 +271,10 @@
     <t>MCP3021</t>
   </si>
   <si>
-    <t xml:space="preserve">U14 </t>
-  </si>
-  <si>
-    <t>MCP23008-xSO</t>
-  </si>
-  <si>
-    <t>C92253</t>
+    <t>Package_TO_SOT_SMD:TSOT-23-5_HandSoldering</t>
+  </si>
+  <si>
+    <t>C128576</t>
   </si>
   <si>
     <t xml:space="preserve">U15 </t>
@@ -184,13 +283,34 @@
     <t>LM339</t>
   </si>
   <si>
-    <t xml:space="preserve">U3 U4 </t>
-  </si>
-  <si>
-    <t>CD4013BPWR</t>
-  </si>
-  <si>
-    <t>C406860</t>
+    <t>Package_SO:SOIC-14_3.9x8.7mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>C7948</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U16 </t>
+  </si>
+  <si>
+    <t>MB85RC256</t>
+  </si>
+  <si>
+    <t>Package_SO:SOIC-8_3.9x4.9mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>C47538</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U3 </t>
+  </si>
+  <si>
+    <t>74LVC07</t>
+  </si>
+  <si>
+    <t>Package_SO:TSSOP-14_4.4x5mm_P0.65mm</t>
+  </si>
+  <si>
+    <t>C7659</t>
   </si>
   <si>
     <t xml:space="preserve">U6 </t>
@@ -199,6 +319,9 @@
     <t>LTC1660CGN</t>
   </si>
   <si>
+    <t>Package_SO:TSSOP-16-1EP_4.4x5mm_P0.65mm</t>
+  </si>
+  <si>
     <t>C676319</t>
   </si>
   <si>
@@ -208,74 +331,17 @@
     <t>LT1790-3.3</t>
   </si>
   <si>
+    <t>Package_TO_SOT_SMD:TSOT-23-6</t>
+  </si>
+  <si>
     <t>C665229</t>
-  </si>
-  <si>
-    <t>C7948</t>
-  </si>
-  <si>
-    <t>C128576</t>
-  </si>
-  <si>
-    <t>C124408</t>
-  </si>
-  <si>
-    <t>J6 J7</t>
-  </si>
-  <si>
-    <t>Conn_02x5_Male</t>
-  </si>
-  <si>
-    <t>0805_C</t>
-  </si>
-  <si>
-    <t>0805_D</t>
-  </si>
-  <si>
-    <t>0805_R</t>
-  </si>
-  <si>
-    <t>SOIC-8</t>
-  </si>
-  <si>
-    <t>TSOT-23-5</t>
-  </si>
-  <si>
-    <t>SOIC-18</t>
-  </si>
-  <si>
-    <t>SOIC-14</t>
-  </si>
-  <si>
-    <t>TSSOP-14</t>
-  </si>
-  <si>
-    <t>TSSOP-16</t>
-  </si>
-  <si>
-    <t>TSOT-23-6</t>
-  </si>
-  <si>
-    <t>Plugin,P=2.54mm</t>
-  </si>
-  <si>
-    <t>C115170</t>
-  </si>
-  <si>
-    <t>332K 1%</t>
-  </si>
-  <si>
-    <t>Cap_SMD</t>
-  </si>
-  <si>
-    <t>C2887276</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -406,6 +472,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -754,9 +828,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1112,39 +1184,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A24" sqref="A24:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.140625" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
-    <col min="3" max="3" width="24.5703125" customWidth="1"/>
-    <col min="4" max="4" width="78.140625" customWidth="1"/>
-    <col min="5" max="5" width="38.85546875" customWidth="1"/>
+    <col min="1" max="1" width="102.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" customWidth="1"/>
+    <col min="4" max="4" width="63.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1155,367 +1227,486 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>82</v>
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>68</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>68</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B5">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>68</v>
+        <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>68</v>
+        <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B7">
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>78</v>
+        <v>29</v>
       </c>
       <c r="E8" t="s">
-        <v>65</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>67</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>78</v>
+        <v>33</v>
       </c>
       <c r="E9" t="s">
-        <v>79</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B10">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>70</v>
+        <v>33</v>
       </c>
       <c r="E10" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>70</v>
+        <v>39</v>
       </c>
       <c r="E11" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B12">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="D12" t="s">
-        <v>70</v>
+        <v>39</v>
       </c>
       <c r="E12" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="B13">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="D13" t="s">
-        <v>70</v>
+        <v>39</v>
       </c>
       <c r="E13" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="B14">
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>80</v>
+        <v>48</v>
       </c>
       <c r="D14" t="s">
-        <v>70</v>
+        <v>39</v>
       </c>
       <c r="E14" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="B15">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" t="s">
         <v>39</v>
       </c>
-      <c r="D15" t="s">
-        <v>70</v>
-      </c>
       <c r="E15" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="D16" t="s">
-        <v>70</v>
+        <v>39</v>
       </c>
       <c r="E16" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="B17">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="D17" t="s">
-        <v>71</v>
+        <v>39</v>
       </c>
       <c r="E17" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="B18">
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="D18" t="s">
-        <v>72</v>
+        <v>39</v>
       </c>
       <c r="E18" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="D19" t="s">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="E19" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="D20" t="s">
-        <v>74</v>
+        <v>39</v>
       </c>
       <c r="E20" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="B21">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="D21" t="s">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="E21" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="D22" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="E22" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="D23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>77</v>
       </c>
-      <c r="E23" t="s">
-        <v>62</v>
+      <c r="B24">
+        <v>11</v>
+      </c>
+      <c r="C24" t="s">
+        <v>78</v>
+      </c>
+      <c r="D24" t="s">
+        <v>79</v>
+      </c>
+      <c r="E24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>81</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25" t="s">
+        <v>82</v>
+      </c>
+      <c r="D25" t="s">
+        <v>83</v>
+      </c>
+      <c r="E25" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>86</v>
+      </c>
+      <c r="D26" t="s">
+        <v>87</v>
+      </c>
+      <c r="E26" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>89</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>90</v>
+      </c>
+      <c r="D27" t="s">
+        <v>91</v>
+      </c>
+      <c r="E27" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>93</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>94</v>
+      </c>
+      <c r="D28" t="s">
+        <v>95</v>
+      </c>
+      <c r="E28" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>97</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>98</v>
+      </c>
+      <c r="D29" t="s">
+        <v>99</v>
+      </c>
+      <c r="E29" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>101</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>102</v>
+      </c>
+      <c r="D30" t="s">
+        <v>103</v>
+      </c>
+      <c r="E30" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>